<commit_message>
Fix all basic functionalities
</commit_message>
<xml_diff>
--- a/test_data/udhr-translations/ro-crate-metadata-w-subcollections2.xlsx
+++ b/test_data/udhr-translations/ro-crate-metadata-w-subcollections2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsw/uqslc/codes/corpus-tools-ro-crate/test_data/udhr-translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA60634E-1E5A-0946-8E00-E0AEAFD3552F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC8BF65-83BD-2442-BD33-DDE72E53376A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="17480" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2480" windowWidth="29920" windowHeight="15680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RootDataset" sheetId="10" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <sheet name="Objects" sheetId="1" r:id="rId10"/>
     <sheet name="Files" sheetId="21" r:id="rId11"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId12"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Objects!$A$1:$H$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">SubCollections!$A$1:$H$4</definedName>
@@ -50,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="189">
   <si>
     <t>@id</t>
   </si>
@@ -598,10 +595,25 @@
     <t>isRef_accountablePerson</t>
   </si>
   <si>
-    <t>[#Danish, #English, #German, #Latin, #Lithuanian, #OldEnglish, #ScottishGaelic, #Welsh]</t>
+    <t>arcp://name,custom/terms#languageStatus</t>
   </si>
   <si>
-    <t>[#AncientEgyptian, #Danish, #English, #Finnish, #German, #Latin, #Lithuanian, #Mongolian, #OldEnglish, #ScottishGaelic, #Welsh]</t>
+    <t>isRef_ldac:hasCollectionProtocol</t>
+  </si>
+  <si>
+    <t>collection.txt</t>
+  </si>
+  <si>
+    <t>ldac:CollectionProtocol</t>
+  </si>
+  <si>
+    <t>Collection Notes</t>
+  </si>
+  <si>
+    <t>#LDaCA</t>
+  </si>
+  <si>
+    <t>Language Data Commons of Australia</t>
   </si>
 </sst>
 </file>
@@ -1283,7 +1295,7 @@
     <xf numFmtId="0" fontId="23" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="26" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1313,6 +1325,9 @@
     <xf numFmtId="0" fontId="32" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="37" borderId="0" xfId="57" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="30" fillId="42" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="58">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1391,54 +1406,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="RootDataset"/>
-      <sheetName val="@context"/>
-      <sheetName val="Custom Terms"/>
-      <sheetName val="Authors"/>
-      <sheetName val="Publishers"/>
-      <sheetName val="Licenses"/>
-      <sheetName val="Provenance"/>
-      <sheetName val="People"/>
-      <sheetName val="Places"/>
-      <sheetName val="Localities"/>
-      <sheetName val="Objects"/>
-      <sheetName val="Files"/>
-      <sheetName val="Schemas"/>
-      <sheetName val="Columns"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="4">
-          <cell r="B4" t="str">
-            <v>arcp://name,custom/terms#</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1738,16 +1705,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1B4B01-7DA1-4F69-8EF2-3B9D5666F67A}">
-  <dimension ref="A1:B16384"/>
+  <dimension ref="A1:B16382"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="111.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="3" bestFit="1" customWidth="1"/>
@@ -1846,43 +1813,38 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="9" t="s">
-        <v>178</v>
+        <v>24</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="9" t="s">
-        <v>179</v>
+      <c r="B14" s="3" t="s">
+        <v>184</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="A15" s="9"/>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="9"/>
@@ -50984,12 +50946,6 @@
     </row>
     <row r="16382" spans="1:1">
       <c r="A16382" s="9"/>
-    </row>
-    <row r="16383" spans="1:1">
-      <c r="A16383" s="9"/>
-    </row>
-    <row r="16384" spans="1:1">
-      <c r="A16384" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -51000,7 +50956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
@@ -51627,11 +51583,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{048E1B1E-E1A3-DF49-8269-1E379487FFDF}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -51643,10 +51599,13 @@
     <col min="5" max="5" width="27.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="24.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="49.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.1640625" style="3"/>
+    <col min="9" max="9" width="11.1640625" style="3"/>
+    <col min="10" max="10" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1">
+    <row r="1" spans="1:11" s="9" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -51671,8 +51630,17 @@
       <c r="H1" s="9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="2" t="str">
         <f>_xlfn.CONCAT(_xlfn.CONCAT(D2,"/"),E2)</f>
         <v>Images/UDHR_AncientEgyptian.png</v>
@@ -51697,7 +51665,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:11">
       <c r="A3" s="2" t="str">
         <f t="shared" ref="A3:A18" si="0">_xlfn.CONCAT(_xlfn.CONCAT(D3,"/"),E3)</f>
         <v>Audio/UDHR_Danish.mp3</v>
@@ -51724,7 +51692,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:11">
       <c r="A4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Text/UDHR_Danish.txt</v>
@@ -51749,7 +51717,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1">
+    <row r="5" spans="1:11" s="4" customFormat="1">
       <c r="A5" s="2" t="str">
         <f t="shared" ref="A5:A11" si="1">_xlfn.CONCAT(_xlfn.CONCAT(D5,"/"),E5)</f>
         <v>Text/UDHR_English.txt</v>
@@ -51773,8 +51741,9 @@
       <c r="H5" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="K5" s="23"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="2" t="str">
         <f t="shared" ref="A6:A7" si="2">_xlfn.CONCAT(_xlfn.CONCAT(D6,"/"),E6)</f>
         <v>Audio/UDHR_Finnish.mp3</v>
@@ -51801,7 +51770,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="4" customFormat="1">
+    <row r="7" spans="1:11" s="4" customFormat="1">
       <c r="A7" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Text/UDHR_Finnish.txt</v>
@@ -51825,8 +51794,9 @@
       <c r="H7" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="K7" s="23"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Audio/UDHR_German.mp3</v>
@@ -51853,7 +51823,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1">
+    <row r="9" spans="1:11" s="4" customFormat="1">
       <c r="A9" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Text/UDHR_German.txt</v>
@@ -51877,8 +51847,9 @@
       <c r="H9" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Audio/UDHR_Icelandic.mp3</v>
@@ -51905,7 +51876,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1">
+    <row r="11" spans="1:11" s="4" customFormat="1">
       <c r="A11" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Text/UDHR_Icelandic.txt</v>
@@ -51929,8 +51900,9 @@
       <c r="H11" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="K11" s="23"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Audio/UDHR_Latin.mp3</v>
@@ -51957,7 +51929,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1">
+    <row r="13" spans="1:11" s="4" customFormat="1">
       <c r="A13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Text/UDHR_Latin.txt</v>
@@ -51981,8 +51953,9 @@
       <c r="H13" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="K13" s="23"/>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Audio/UDHR_Lithuanian.mp3</v>
@@ -52009,7 +51982,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1">
+    <row r="15" spans="1:11" s="4" customFormat="1">
       <c r="A15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Text/UDHR_Lithuanian.txt</v>
@@ -52033,8 +52006,9 @@
       <c r="H15" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="K15" s="23"/>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="2" t="str">
         <f t="shared" ref="A16:A17" si="3">_xlfn.CONCAT(_xlfn.CONCAT(D16,"/"),E16)</f>
         <v>Audio/UDHR_Mongolian.mp3</v>
@@ -52061,7 +52035,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="4" customFormat="1">
+    <row r="17" spans="1:11" s="4" customFormat="1">
       <c r="A17" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Text/UDHR_Mongolian.txt</v>
@@ -52085,8 +52059,9 @@
       <c r="H17" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" s="4" customFormat="1">
+      <c r="K17" s="23"/>
+    </row>
+    <row r="18" spans="1:11" s="4" customFormat="1">
       <c r="A18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Images/UDHR_OldEnglish.png</v>
@@ -52110,8 +52085,9 @@
       <c r="H18" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" s="4" customFormat="1">
+      <c r="K18" s="23"/>
+    </row>
+    <row r="19" spans="1:11" s="4" customFormat="1">
       <c r="A19" s="2" t="str">
         <f t="shared" ref="A19:A21" si="4">_xlfn.CONCAT(_xlfn.CONCAT(D19,"/"),E19)</f>
         <v>Text/UDHR_OldEnglish.txt</v>
@@ -52135,8 +52111,9 @@
       <c r="H19" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" s="4" customFormat="1">
+      <c r="K19" s="23"/>
+    </row>
+    <row r="20" spans="1:11" s="4" customFormat="1">
       <c r="A20" s="2" t="str">
         <f t="shared" si="4"/>
         <v>Audio/UDHR_ScottishGaelic.mp3</v>
@@ -52162,8 +52139,9 @@
       <c r="H20" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" s="4" customFormat="1">
+      <c r="K20" s="23"/>
+    </row>
+    <row r="21" spans="1:11" s="4" customFormat="1">
       <c r="A21" s="2" t="str">
         <f t="shared" si="4"/>
         <v>Text/UDHR_ScottishGaelic.txt</v>
@@ -52187,8 +52165,9 @@
       <c r="H21" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" s="4" customFormat="1">
+      <c r="K21" s="23"/>
+    </row>
+    <row r="22" spans="1:11" s="4" customFormat="1">
       <c r="A22" s="2" t="str">
         <f t="shared" ref="A22:A23" si="5">_xlfn.CONCAT(_xlfn.CONCAT(D22,"/"),E22)</f>
         <v>Audio/UDHR_Welsh.mp3</v>
@@ -52214,8 +52193,9 @@
       <c r="H22" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" s="4" customFormat="1">
+      <c r="K22" s="23"/>
+    </row>
+    <row r="23" spans="1:11" s="4" customFormat="1">
       <c r="A23" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Text/UDHR_Welsh.txt</v>
@@ -52238,6 +52218,27 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
         <v>107</v>
+      </c>
+      <c r="K23" s="23"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K24" s="22" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -52339,9 +52340,8 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="2" t="str">
-        <f>_xlfn.CONCAT('[1]@context'!B4, B2)</f>
-        <v>arcp://name,custom/terms#languageStatus</v>
+      <c r="A2" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>95</v>
@@ -52360,9 +52360,8 @@
       <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="2" t="str">
-        <f>_xlfn.CONCAT('[1]@context'!B4, B3)</f>
-        <v>arcp://name,custom/terms#Extinct</v>
+      <c r="A3" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>96</v>
@@ -52383,9 +52382,8 @@
       <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="2" t="str">
-        <f>_xlfn.CONCAT('[1]@context'!B4, B4)</f>
-        <v>arcp://name,custom/terms#Living</v>
+      <c r="A4" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>98</v>
@@ -52406,9 +52404,8 @@
       <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="2" t="str">
-        <f>_xlfn.CONCAT('[1]@context'!B4, B5)</f>
-        <v>arcp://name,custom/terms#LanguageStatusTerms</v>
+      <c r="A5" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>97</v>
@@ -52434,11 +52431,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9114C3-3381-1A44-A5FD-3E1188129C58}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -52469,6 +52466,17 @@
       </c>
       <c r="C2" s="1" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -53042,11 +53050,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7D76345-DBE6-934F-BA9B-7F1970C9CBCC}">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -53059,12 +53067,11 @@
     <col min="6" max="6" width="25.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42.5" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.33203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="26.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.1640625" style="3"/>
+    <col min="9" max="9" width="26.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1">
+    <row r="1" spans="1:9" s="9" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -53090,13 +53097,10 @@
         <v>27</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="J1" s="9" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="str">
         <f>_xlfn.CONCAT("#",C2)</f>
         <v>#Afro-Asiatic</v>
@@ -53122,13 +53126,10 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="J2" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="str">
         <f>_xlfn.CONCAT("#",C3)</f>
         <v>#Indo-European</v>
@@ -53154,13 +53155,10 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="J3" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="str">
         <f>_xlfn.CONCAT("#",C4)</f>
         <v>#Mongolic</v>
@@ -53186,13 +53184,10 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="J4" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="str">
         <f>_xlfn.CONCAT("#",C5)</f>
         <v>#Uralic</v>
@@ -53218,63 +53213,60 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J5" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:9">
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:9">
       <c r="E7" s="7"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:9">
       <c r="E8" s="7"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:9">
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:9">
       <c r="E10" s="7"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:9">
       <c r="E11" s="7"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:9">
       <c r="E12" s="7"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:9">
       <c r="E13" s="7"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:9">
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:9">
       <c r="E15" s="7"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:9">
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>

</xml_diff>